<commit_message>
Cleaned code and updated challenge 4 & 5 excel files
</commit_message>
<xml_diff>
--- a/Challenges/Challenge 4/Challenge 4 - Pluto's Orbit.xlsx
+++ b/Challenges/Challenge 4/Challenge 4 - Pluto's Orbit.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\vidis\Desktop\BPhO\Challenges\Challenge 4\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DF089F03-82CA-45AA-AECF-D1DD43D26CEC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5941BF27-7A48-432B-BC46-3C174C38D25C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{4AEBF47C-BD5F-49ED-8FB0-CE97F789EC3D}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
   <si>
     <t>Pluto x</t>
   </si>
@@ -52,14 +52,27 @@
   <si>
     <t>py</t>
   </si>
+  <si>
+    <t>shows pluto in the solar system at an orbital inclination of 17.5 degrees</t>
+  </si>
+  <si>
+    <t>I used excel to complete this challenge and created a graph that</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="15"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -86,9 +99,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1538,7 +1552,7 @@
   <dimension ref="A1:AL24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N18" sqref="N18"/>
+      <selection activeCell="J24" sqref="J24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2224,6 +2238,16 @@
       <c r="S17" s="1"/>
       <c r="AK17" s="1"/>
     </row>
+    <row r="20" spans="10:37" ht="19.5" x14ac:dyDescent="0.3">
+      <c r="J20" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="21" spans="10:37" ht="19.5" x14ac:dyDescent="0.3">
+      <c r="J21" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
     <row r="23" spans="10:37" x14ac:dyDescent="0.25">
       <c r="J23" s="1"/>
       <c r="AB23" s="1"/>
@@ -2234,6 +2258,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId1"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>